<commit_message>
Modification de GANTT, tableau_niveau, et PERT
</commit_message>
<xml_diff>
--- a/Gestion_projet/PERT/Tableau_niveau.xlsx
+++ b/Gestion_projet/PERT/Tableau_niveau.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bureau\Cours\URCA\Projet\Projet S2\PERT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bureau\Cours\URCA\Projet\Projet S2\infs2_prj06\Gestion_projet\PERT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34FB846-2D6E-40B3-B3B8-4DAA62FCAA51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5892D222-06A3-448F-8202-DEBB0CBEE17F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17064" yWindow="672" windowWidth="11520" windowHeight="7020" xr2:uid="{8642F586-A4CB-4C98-B4EF-2AB57138F504}"/>
+    <workbookView xWindow="7692" yWindow="-108" windowWidth="22968" windowHeight="7020" xr2:uid="{8642F586-A4CB-4C98-B4EF-2AB57138F504}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
-  <si>
-    <t>T</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="51">
   <si>
     <t>A</t>
   </si>
@@ -45,12 +42,6 @@
     <t>I</t>
   </si>
   <si>
-    <t>I, K</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
     <t>Niveau</t>
   </si>
   <si>
@@ -96,9 +87,6 @@
     <t>P</t>
   </si>
   <si>
-    <t>Analyse des besoins</t>
-  </si>
-  <si>
     <t>Rédaction du cahier des charges</t>
   </si>
   <si>
@@ -108,75 +96,18 @@
     <t>Rédaction du plan projet</t>
   </si>
   <si>
-    <t>Organisation de l'équipe</t>
-  </si>
-  <si>
-    <t>Validation du plan projet</t>
-  </si>
-  <si>
-    <t>Enchaînement des grilles écrans</t>
-  </si>
-  <si>
-    <t>Présentation des pages écrans</t>
-  </si>
-  <si>
-    <t>Validation des enchaînements et de la présentation des écrans</t>
-  </si>
-  <si>
     <t>Analyse des spécifications fonctionnelles</t>
   </si>
   <si>
     <t>Rédaction des spécifications fonctionnelles</t>
   </si>
   <si>
-    <t>Architecture logicielle</t>
-  </si>
-  <si>
-    <t>Maquette</t>
-  </si>
-  <si>
-    <t>Validation de la conception visuelle et des spécifications techniques</t>
-  </si>
-  <si>
     <t>Développement de l'IHM</t>
   </si>
   <si>
-    <t>Interfaçage à une base de données</t>
-  </si>
-  <si>
-    <t>Programmation des fonctionnalités du site</t>
-  </si>
-  <si>
-    <t>Tests en interne</t>
-  </si>
-  <si>
-    <t>Validation de la phase de réalisation</t>
-  </si>
-  <si>
     <t>/</t>
   </si>
   <si>
-    <t>A, B</t>
-  </si>
-  <si>
-    <t>F (FF)</t>
-  </si>
-  <si>
-    <t>G, H</t>
-  </si>
-  <si>
-    <t>C, F</t>
-  </si>
-  <si>
-    <t>K, M</t>
-  </si>
-  <si>
-    <t>I, N</t>
-  </si>
-  <si>
-    <t>P, Q, R</t>
-  </si>
-  <si>
     <t>Q</t>
   </si>
   <si>
@@ -184,15 +115,6 @@
   </si>
   <si>
     <t>Durée</t>
-  </si>
-  <si>
-    <t>O,P,Q,R</t>
-  </si>
-  <si>
-    <t>F, E (F FF)</t>
-  </si>
-  <si>
-    <t>G, L, M, J, H</t>
   </si>
   <si>
     <t xml:space="preserve">jalon </t>
@@ -222,7 +144,61 @@
     </r>
   </si>
   <si>
-    <t>Hébergement du site et de la base de donnée</t>
+    <t>Analyse fonctionnelle</t>
+  </si>
+  <si>
+    <t>Validation du plan projet et de l'organisation de l'équipe</t>
+  </si>
+  <si>
+    <t>Détermination de la structure des écrans</t>
+  </si>
+  <si>
+    <t>Validation de la structure des écrans</t>
+  </si>
+  <si>
+    <t>jalon</t>
+  </si>
+  <si>
+    <t>C, E</t>
+  </si>
+  <si>
+    <t>Architecture logicielle: découpage du site en modules</t>
+  </si>
+  <si>
+    <t>Recherche du contenu de la base de données</t>
+  </si>
+  <si>
+    <t>Création de la maquette du site</t>
+  </si>
+  <si>
+    <t>Validation de la maquette et du principe de navigation du site</t>
+  </si>
+  <si>
+    <t>Développement de la base de données</t>
+  </si>
+  <si>
+    <t>Développement des fonctionnalités du site</t>
+  </si>
+  <si>
+    <t>Tests sur le bon fonctionnement du site web</t>
+  </si>
+  <si>
+    <t>N, O, P</t>
+  </si>
+  <si>
+    <t>F, H, J, K, L</t>
+  </si>
+  <si>
+    <t>G, I</t>
+  </si>
+  <si>
+    <t>Validation de la phase de réalisation et hébergement du site</t>
+  </si>
+  <si>
+    <t>et de la base de données</t>
+  </si>
+  <si>
+    <t>L, I, G</t>
   </si>
 </sst>
 </file>
@@ -302,7 +278,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -379,13 +355,98 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -423,6 +484,36 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20 % - Accent1" xfId="2" builtinId="30"/>
@@ -739,16 +830,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E96C0C06-AB2E-4D32-8E6B-4BD5B0942B9E}">
-  <dimension ref="A2:D39"/>
+  <dimension ref="A2:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.109375" customWidth="1"/>
-    <col min="2" max="2" width="55.77734375" customWidth="1"/>
+    <col min="2" max="2" width="50.44140625" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
     <col min="5" max="5" width="5.33203125" customWidth="1"/>
     <col min="6" max="6" width="8.109375" customWidth="1"/>
@@ -759,32 +850,32 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B2" s="14" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="D5" s="9">
         <v>1</v>
@@ -792,13 +883,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="9">
         <v>1</v>
@@ -806,27 +897,27 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" s="9">
         <v>1</v>
@@ -834,55 +925,55 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="9">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>56</v>
+        <v>37</v>
+      </c>
+      <c r="D10" s="9">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="9">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D12" s="9">
         <v>1</v>
@@ -890,27 +981,27 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>56</v>
+        <v>12</v>
+      </c>
+      <c r="D13" s="9">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D14" s="9">
         <v>1</v>
@@ -918,13 +1009,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="D15" s="9">
         <v>1</v>
@@ -932,141 +1023,135 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D16" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="9">
-        <v>2</v>
+        <v>50</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>56</v>
+        <v>16</v>
+      </c>
+      <c r="D18" s="9">
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D19" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="D20" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="6" t="s">
+      <c r="A21" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" s="9">
-        <v>3</v>
+      <c r="C22" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="6" t="s">
+      <c r="A23" s="28"/>
+      <c r="B23" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="9">
+      <c r="C23" s="26"/>
+      <c r="D23" s="23"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="15"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="17"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+      <c r="B28" s="10" t="s">
         <v>0</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>1</v>
@@ -1074,7 +1159,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B30" s="10" t="s">
         <v>2</v>
@@ -1082,7 +1167,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B31" s="10" t="s">
         <v>3</v>
@@ -1090,66 +1175,58 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="1">
-        <v>9</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>53</v>
+      <c r="A37" s="7">
+        <v>10</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="7">
-        <v>10</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="8">
+      <c r="A38" s="8">
         <v>11</v>
       </c>
-      <c r="B39" s="12" t="s">
-        <v>0</v>
+      <c r="B38" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>